<commit_message>
Added new classes to handle better differences between types.
Error processing is managed during generation, with a specific display (MessageBox of Excel).
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Target</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>STEP 2</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>STEP 3</t>
   </si>
 </sst>
 </file>
@@ -262,23 +271,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:D9" totalsRowCount="1">
-  <autoFilter ref="B5:D8"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F9" totalsRowCount="1">
+  <autoFilter ref="B5:F8"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
+    <tableColumn id="4" name="STEP 2"/>
+    <tableColumn id="5" name="STEP 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B11:D12" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B11:F12" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="5">
     <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="4" name="Colonne1"/>
+    <tableColumn id="5" name="Colonne2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -597,10 +610,10 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +623,7 @@
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -618,7 +631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -626,7 +639,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -637,10 +650,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -653,8 +666,14 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -665,8 +684,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>14</v>
@@ -677,8 +702,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -688,8 +716,11 @@
       <c r="D8">
         <v>2000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,7 +728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
@@ -707,8 +738,11 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
@@ -719,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Completed all templates, already implemented.
Added interfaces.
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Target</t>
   </si>
@@ -68,6 +68,21 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>STEP 2</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>R:R_Pressure</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>STEP 3</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,6 +147,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -164,6 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,23 +284,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:D9" totalsRowCount="1">
-  <autoFilter ref="B5:D8"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F10" totalsRowCount="1">
+  <autoFilter ref="B5:F9"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
+    <tableColumn id="4" name="STEP 2" totalsRowLabel="400"/>
+    <tableColumn id="5" name="STEP 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B11:D12" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B12:F14" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="5">
     <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="4" name="Column1"/>
+    <tableColumn id="5" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -289,7 +315,7 @@
   <tableColumns count="15">
     <tableColumn id="1" name="Colonne1"/>
     <tableColumn id="2" name="Colonne2"/>
-    <tableColumn id="3" name="Colonne3"/>
+    <tableColumn id="16" name="Column1"/>
     <tableColumn id="4" name="Colonne4"/>
     <tableColumn id="5" name="Colonne5"/>
     <tableColumn id="6" name="Colonne6"/>
@@ -308,7 +334,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,36 +623,42 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -636,11 +668,14 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -653,8 +688,14 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>10</v>
@@ -665,8 +706,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>14</v>
@@ -677,8 +724,14 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -688,39 +741,85 @@
       <c r="D8">
         <v>2000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="E8">
+        <v>450</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>1.5</v>
+      </c>
+      <c r="E9">
+        <v>2.8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>2.8</v>
+      </c>
+      <c r="E14">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to use forcing of elements of array.
Added ability to skip, force fail, force passed an individual instruction, or a complete line.

Updated test sequence to reflect those changes.
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Target</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans1</t>
   </si>
   <si>
-    <t>B_CabAct</t>
-  </si>
-  <si>
     <t>B_HHTOpenState_Veh1_DDU</t>
   </si>
   <si>
@@ -83,6 +80,48 @@
   </si>
   <si>
     <t>STEP 3</t>
+  </si>
+  <si>
+    <t>{PF}B_CabAct</t>
+  </si>
+  <si>
+    <t>{PF}1</t>
+  </si>
+  <si>
+    <t>{S}450</t>
+  </si>
+  <si>
+    <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans2</t>
+  </si>
+  <si>
+    <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans3</t>
+  </si>
+  <si>
+    <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans4</t>
+  </si>
+  <si>
+    <t>Application_TrTrans/Embedded/Control_Command/FBS/TFE/tfe_aht_trtrans1/tfe_aht_f15_trtrans5</t>
+  </si>
+  <si>
+    <t>Variable[3]</t>
+  </si>
+  <si>
+    <t>I:Variable[3]</t>
+  </si>
+  <si>
+    <t>R:Variable[3]</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Variable[2]</t>
+  </si>
+  <si>
+    <t>R:Variable[2]</t>
   </si>
 </sst>
 </file>
@@ -182,18 +221,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -208,6 +244,9 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -284,10 +323,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F10" totalsRowCount="1">
-  <autoFilter ref="B5:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F16" totalsRowCount="1">
+  <autoFilter ref="B5:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
     <tableColumn id="4" name="STEP 2" totalsRowLabel="400"/>
@@ -298,11 +337,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B12:F14" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B18:F23" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="Target" dataDxfId="2"/>
+    <tableColumn id="1" name="Target" dataDxfId="1"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="0"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -334,7 +373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -623,13 +662,13 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -641,10 +680,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -652,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,7 +715,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -689,16 +728,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -710,30 +749,30 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>23</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -741,16 +780,16 @@
       <c r="D8">
         <v>2000</v>
       </c>
-      <c r="E8">
-        <v>450</v>
+      <c r="E8" t="s">
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>20</v>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -762,65 +801,162 @@
         <v>2.8</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>-20.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D20">
+        <v>2.8</v>
+      </c>
+      <c r="E20">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21">
         <v>10</v>
       </c>
-      <c r="E12">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22">
         <v>-25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14">
-        <v>2.8</v>
-      </c>
-      <c r="E14">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
         <v>-1.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="42" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added possibility to use popups in check steps.
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Target</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>This is my message</t>
+  </si>
+  <si>
+    <t>This is my message 2</t>
   </si>
 </sst>
 </file>
@@ -228,18 +231,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -254,6 +254,9 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -333,7 +336,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F17" totalsRowCount="1">
   <autoFilter ref="B5:F16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
     <tableColumn id="4" name="STEP 2" totalsRowLabel="400"/>
@@ -344,11 +347,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:F24" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:F25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="Target" dataDxfId="2"/>
+    <tableColumn id="1" name="Target" dataDxfId="1"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="0"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -669,10 +672,10 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +725,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -742,7 +745,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -760,7 +763,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -878,7 +881,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D16" t="s">
@@ -929,48 +932,56 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21">
-        <v>2.8</v>
-      </c>
-      <c r="E21">
-        <v>-1.7</v>
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>2.8</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-1.7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23">
-        <v>-25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>-1.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New template with handling of multiple unit.
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Target</t>
   </si>
@@ -131,6 +131,33 @@
   </si>
   <si>
     <t>This is my message 2</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Unit1/MPU1</t>
+  </si>
+  <si>
+    <t>Unit1/MPU2</t>
+  </si>
+  <si>
+    <t>Unit2/MPU1</t>
+  </si>
+  <si>
+    <t>Unit2/MPU2</t>
+  </si>
+  <si>
+    <t>Unit1/ENV</t>
+  </si>
+  <si>
+    <t>Unit2/ENV</t>
+  </si>
+  <si>
+    <t>Unit3/ENV</t>
+  </si>
+  <si>
+    <t>Unit4/ENV</t>
   </si>
 </sst>
 </file>
@@ -241,6 +268,9 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -254,9 +284,6 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -333,11 +360,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:F17" totalsRowCount="1">
-  <autoFilter ref="B5:F16"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="Location"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
+  <autoFilter ref="B5:G16"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Path"/>
+    <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
     <tableColumn id="4" name="STEP 2" totalsRowLabel="400"/>
     <tableColumn id="5" name="STEP 3"/>
@@ -347,11 +375,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:F25" headerRowCount="0" totalsRowShown="0">
-  <tableColumns count="5">
-    <tableColumn id="1" name="Target" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="0"/>
+    <tableColumn id="6" name="Colonne1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -672,10 +701,10 @@
   <sheetPr codeName="Feuil4">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,9 +712,10 @@
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -696,7 +726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -707,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -721,10 +751,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -732,19 +762,22 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>22</v>
@@ -752,17 +785,20 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" t="s">
         <v>13</v>
@@ -771,50 +807,59 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
         <v>2000</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9">
         <v>1.5</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2.8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
@@ -822,32 +867,41 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
@@ -855,79 +909,94 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
         <v>-20.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>-25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -935,53 +1004,68 @@
         <v>36</v>
       </c>
       <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
         <v>2.8</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>-1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="E23">
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="E24">
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24">
         <v>-25</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="E25">
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25">
         <v>-1.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Proposal for version 0.0.4
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
   </bookViews>
   <sheets>
-    <sheet name="Test_1.2" sheetId="4" r:id="rId1"/>
+    <sheet name="TEST_1.1" sheetId="5" r:id="rId1"/>
+    <sheet name="Test_1.2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="53">
   <si>
     <t>Target</t>
   </si>
@@ -158,6 +159,22 @@
   </si>
   <si>
     <t>Unit4/ENV</t>
+  </si>
+  <si>
+    <t>Test 1.1</t>
+  </si>
+  <si>
+    <t>{P}B_CabAct</t>
+  </si>
+  <si>
+    <t>{F}1</t>
+  </si>
+  <si>
+    <t>This is my message with "forbidden characters"</t>
+  </si>
+  <si>
+    <t>This is my message 2 :
+"It BREAKS!"</t>
   </si>
 </sst>
 </file>
@@ -241,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -262,11 +279,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -284,6 +307,36 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -344,11 +397,11 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Description table" pivot="0" count="5">
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstColumn" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="4"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -360,7 +413,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
@@ -375,7 +428,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
     <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
@@ -389,6 +442,58 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table_Desc_1.1" displayName="Table_Desc_1.1" ref="C1:Q4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="15">
+    <tableColumn id="1" name="Colonne1"/>
+    <tableColumn id="2" name="Colonne2"/>
+    <tableColumn id="16" name="Column1"/>
+    <tableColumn id="4" name="Colonne4"/>
+    <tableColumn id="5" name="Colonne5"/>
+    <tableColumn id="6" name="Colonne6"/>
+    <tableColumn id="7" name="Colonne7"/>
+    <tableColumn id="8" name="Colonne8"/>
+    <tableColumn id="9" name="Colonne9"/>
+    <tableColumn id="10" name="Colonne10"/>
+    <tableColumn id="11" name="Colonne11"/>
+    <tableColumn id="12" name="Colonne12"/>
+    <tableColumn id="13" name="Colonne13"/>
+    <tableColumn id="14" name="Colonne14"/>
+    <tableColumn id="15" name="Colonne15"/>
+  </tableColumns>
+  <tableStyleInfo name="Description table" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
+  <autoFilter ref="B5:G16"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Path"/>
+    <tableColumn id="6" name="Location"/>
+    <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
+    <tableColumn id="4" name="STEP 2" totalsRowLabel="400"/>
+    <tableColumn id="5" name="STEP 3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Target" dataDxfId="5"/>
+    <tableColumn id="2" name="Location"/>
+    <tableColumn id="6" name="Colonne1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="4"/>
+    <tableColumn id="4" name="Column1"/>
+    <tableColumn id="5" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table_Desc_1.2" displayName="Table_Desc_1.2" ref="C1:Q4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="15">
     <tableColumn id="1" name="Colonne1"/>
@@ -698,13 +803,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Feuil4">
-    <tabColor theme="3"/>
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>2000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9">
+        <v>1.5</v>
+      </c>
+      <c r="F9">
+        <v>2.8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>-20.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>2.8</v>
+      </c>
+      <c r="F22">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25">
+        <v>-1.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil4">
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +1244,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -778,7 +1267,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -799,7 +1288,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Added multiple unit support (basic).
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -7,10 +7,11 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_1.1" sheetId="5" r:id="rId1"/>
+    <sheet name="Test_1.1" sheetId="5" r:id="rId1"/>
     <sheet name="Test_1.2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -279,11 +280,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -307,6 +308,9 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -334,9 +338,6 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -416,7 +417,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -430,10 +431,10 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="2"/>
+    <tableColumn id="1" name="Target" dataDxfId="6"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="5"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -468,7 +469,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="4" totalsRowDxfId="3"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -482,10 +483,10 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="5"/>
+    <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="4"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -809,7 +810,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D11" sqref="D11:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +862,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -884,7 +885,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>49</v>
       </c>
@@ -905,7 +906,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1015,7 +1016,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1029,7 +1030,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14">
         <v>-5</v>
@@ -1043,7 +1044,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15">
         <v>-20.8</v>
@@ -1109,7 +1110,7 @@
       <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1244,7 +1245,7 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1267,7 +1268,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1288,7 +1289,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Correction if ticket #63.
</commit_message>
<xml_diff>
--- a/test/UnitTest 2013 00.xlsx
+++ b/test/UnitTest 2013 00.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19980" windowHeight="8070" tabRatio="258" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test_1.1" sheetId="5" r:id="rId1"/>
     <sheet name="Test_1.2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>Target</t>
   </si>
@@ -154,12 +153,6 @@
   </si>
   <si>
     <t>Unit2/ENV</t>
-  </si>
-  <si>
-    <t>Unit3/ENV</t>
-  </si>
-  <si>
-    <t>Unit4/ENV</t>
   </si>
   <si>
     <t>Test 1.1</t>
@@ -176,6 +169,30 @@
   <si>
     <t>This is my message 2 :
 "It BREAKS!"</t>
+  </si>
+  <si>
+    <t>Section1/MPU_A</t>
+  </si>
+  <si>
+    <t>Section2/MPU_A</t>
+  </si>
+  <si>
+    <t>Section1/MPU_T</t>
+  </si>
+  <si>
+    <t>Section2/MPU_T</t>
+  </si>
+  <si>
+    <t>Section1/ENV</t>
+  </si>
+  <si>
+    <t>Section2/ENV</t>
+  </si>
+  <si>
+    <t>Section3/ENV</t>
+  </si>
+  <si>
+    <t>Section4/ENV</t>
   </si>
 </sst>
 </file>
@@ -310,9 +327,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <color theme="0"/>
@@ -338,6 +352,9 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -417,7 +434,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_Action_1.1" displayName="Table_Action_1.1" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -431,10 +448,10 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_Check_1.1" displayName="Table_Check_1.1" ref="B19:G25" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" dataDxfId="6"/>
+    <tableColumn id="1" name="Target" dataDxfId="5"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="6" name="Colonne1"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="5"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="4"/>
     <tableColumn id="4" name="Column1"/>
     <tableColumn id="5" name="Column2"/>
   </tableColumns>
@@ -469,7 +486,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:G17" totalsRowCount="1">
   <autoFilter ref="B5:G16"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Path"/>
     <tableColumn id="6" name="Location"/>
     <tableColumn id="3" name="STEP 1" totalsRowLabel="200"/>
@@ -518,7 +535,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -809,11 +826,11 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -846,7 +863,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -887,7 +904,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -917,7 +934,7 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -1055,7 +1072,7 @@
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,7 +1128,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,11 +1210,11 @@
   </sheetPr>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -1276,7 +1293,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1297,7 +1314,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -1317,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>2000</v>
@@ -1337,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E9">
         <v>1.5</v>
@@ -1357,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -1371,7 +1388,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -1385,7 +1402,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1399,7 +1416,7 @@
         <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>32</v>
@@ -1413,7 +1430,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>-5</v>
@@ -1427,7 +1444,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E15">
         <v>-20.8</v>
@@ -1460,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E19">
         <v>10</v>
@@ -1477,7 +1494,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1493,9 +1510,6 @@
       <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
-        <v>42</v>
-      </c>
       <c r="E21" t="s">
         <v>38</v>
       </c>
@@ -1508,7 +1522,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E22">
         <v>2.8</v>
@@ -1525,7 +1539,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1539,7 +1553,7 @@
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F24">
         <v>-25</v>
@@ -1553,7 +1567,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F25">
         <v>-1.7</v>

</xml_diff>